<commit_message>
Adicionando as notas da Lais
</commit_message>
<xml_diff>
--- a/get170/TurmaB1_semNome.xlsx
+++ b/get170/TurmaB1_semNome.xlsx
@@ -353,7 +353,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -377,12 +377,8 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -403,36 +399,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF5B9BD5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -503,33 +486,33 @@
   </sheetPr>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.0816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="11.7908163265306"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="2" width="13.6785714285714"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1022" min="8" style="2" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="2" width="14.219387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.35714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1022" min="8" style="2" width="9.35714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="9.35714285714286"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="0.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="33.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -545,20 +528,20 @@
       <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -578,7 +561,7 @@
       <c r="F3" s="2" t="n">
         <v>7.5</v>
       </c>
-      <c r="G3" s="5" t="n">
+      <c r="G3" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H3" s="2" t="n">
@@ -590,7 +573,7 @@
         <v>9.75</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -610,7 +593,7 @@
       <c r="F4" s="2" t="n">
         <v>6.75</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H4" s="2" t="n">
@@ -622,7 +605,7 @@
         <v>8.15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -642,7 +625,7 @@
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="2" t="n">
@@ -654,7 +637,7 @@
         <v>4.28</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -669,8 +652,8 @@
         <f aca="false">IF(C6+D6 &lt;= 10,C6+D6,10)</f>
         <v>2</v>
       </c>
-      <c r="F6" s="0"/>
-      <c r="G6" s="5" t="n">
+      <c r="F6" s="5"/>
+      <c r="G6" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H6" s="2" t="n">
@@ -682,7 +665,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -702,7 +685,7 @@
       <c r="F7" s="2" t="n">
         <v>8.25</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H7" s="2" t="n">
@@ -714,7 +697,7 @@
         <v>6.53</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -729,8 +712,8 @@
         <f aca="false">IF(C8+D8 &lt;= 10,C8+D8,10)</f>
         <v>2</v>
       </c>
-      <c r="F8" s="0"/>
-      <c r="G8" s="5" t="n">
+      <c r="F8" s="5"/>
+      <c r="G8" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H8" s="2" t="n">
@@ -742,7 +725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -757,8 +740,8 @@
         <f aca="false">IF(C9+D9 &lt;= 10,C9+D9,10)</f>
         <v>2</v>
       </c>
-      <c r="F9" s="0"/>
-      <c r="G9" s="5" t="n">
+      <c r="F9" s="5"/>
+      <c r="G9" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H9" s="2" t="n">
@@ -770,7 +753,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -788,7 +771,7 @@
       <c r="F10" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G10" s="5" t="n">
+      <c r="G10" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H10" s="2" t="n">
@@ -800,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
@@ -817,8 +800,8 @@
         <f aca="false">IF(C11+D11 &lt;= 10,C11+D11,10)</f>
         <v>3.05</v>
       </c>
-      <c r="F11" s="0"/>
-      <c r="G11" s="5" t="n">
+      <c r="F11" s="5"/>
+      <c r="G11" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H11" s="2" t="n">
@@ -830,7 +813,7 @@
         <v>2.53</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
@@ -850,7 +833,7 @@
       <c r="F12" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H12" s="2" t="n">
@@ -862,7 +845,7 @@
         <v>8.35</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
@@ -877,8 +860,8 @@
         <f aca="false">IF(C13+D13 &lt;= 10,C13+D13,10)</f>
         <v>2</v>
       </c>
-      <c r="F13" s="0"/>
-      <c r="G13" s="5" t="n">
+      <c r="F13" s="5"/>
+      <c r="G13" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H13" s="2" t="n">
@@ -890,7 +873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
         <v>30</v>
       </c>
@@ -905,8 +888,8 @@
         <f aca="false">IF(C14+D14 &lt;= 10,C14+D14,10)</f>
         <v>2</v>
       </c>
-      <c r="F14" s="0"/>
-      <c r="G14" s="5" t="n">
+      <c r="F14" s="5"/>
+      <c r="G14" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H14" s="2" t="n">
@@ -918,7 +901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>32</v>
       </c>
@@ -938,7 +921,7 @@
       <c r="F15" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H15" s="2" t="n">
@@ -950,7 +933,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
         <v>34</v>
       </c>
@@ -970,7 +953,7 @@
       <c r="F16" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H16" s="2" t="n">
@@ -982,7 +965,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
         <v>36</v>
       </c>
@@ -990,19 +973,19 @@
         <v>37</v>
       </c>
       <c r="C17" s="4" t="n">
-        <v>0</v>
+        <v>4.25</v>
       </c>
       <c r="D17" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E17" s="4" t="n">
         <f aca="false">IF(C17+D17 &lt;= 10,C17+D17,10)</f>
-        <v>2</v>
+        <v>6.25</v>
       </c>
       <c r="F17" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H17" s="2" t="n">
@@ -1011,38 +994,42 @@
       </c>
       <c r="I17" s="2" t="n">
         <f aca="false">ROUND((E17+H17)/2,2)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>8.13</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="n">
+        <v>6.2</v>
+      </c>
       <c r="D18" s="4" t="n">
         <v>2</v>
       </c>
       <c r="E18" s="4" t="n">
         <f aca="false">IF(C18+D18 &lt;= 10,C18+D18,10)</f>
-        <v>2</v>
-      </c>
-      <c r="F18" s="0"/>
-      <c r="G18" s="5" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="G18" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H18" s="2" t="n">
         <f aca="false">IF(F18+G18 &lt;= 10,F18+G18,10)</f>
-        <v>2</v>
+        <v>9.4</v>
       </c>
       <c r="I18" s="2" t="n">
         <f aca="false">ROUND((E18+H18)/2,2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>8.8</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>40</v>
       </c>
@@ -1062,7 +1049,7 @@
       <c r="F19" s="2" t="n">
         <v>4.65</v>
       </c>
-      <c r="G19" s="5" t="n">
+      <c r="G19" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H19" s="2" t="n">
@@ -1074,7 +1061,7 @@
         <v>5.23</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
         <v>42</v>
       </c>
@@ -1089,8 +1076,8 @@
         <f aca="false">IF(C20+D20 &lt;= 10,C20+D20,10)</f>
         <v>2</v>
       </c>
-      <c r="F20" s="0"/>
-      <c r="G20" s="5" t="n">
+      <c r="F20" s="5"/>
+      <c r="G20" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H20" s="2" t="n">
@@ -1102,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
         <v>44</v>
       </c>
@@ -1122,7 +1109,7 @@
       <c r="F21" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H21" s="2" t="n">
@@ -1134,7 +1121,7 @@
         <v>4.9</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
         <v>46</v>
       </c>
@@ -1152,7 +1139,7 @@
       <c r="F22" s="2" t="n">
         <v>5.5</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H22" s="2" t="n">
@@ -1164,7 +1151,7 @@
         <v>4.75</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
         <v>48</v>
       </c>
@@ -1184,7 +1171,7 @@
       <c r="F23" s="2" t="n">
         <v>4.9</v>
       </c>
-      <c r="G23" s="5" t="n">
+      <c r="G23" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H23" s="2" t="n">
@@ -1196,7 +1183,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -1216,7 +1203,7 @@
       <c r="F24" s="2" t="n">
         <v>9.75</v>
       </c>
-      <c r="G24" s="5" t="n">
+      <c r="G24" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H24" s="2" t="n">
@@ -1228,7 +1215,7 @@
         <v>8.8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -1243,8 +1230,8 @@
         <f aca="false">IF(C25+D25 &lt;= 10,C25+D25,10)</f>
         <v>2</v>
       </c>
-      <c r="F25" s="0"/>
-      <c r="G25" s="5" t="n">
+      <c r="F25" s="5"/>
+      <c r="G25" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H25" s="2" t="n">
@@ -1256,7 +1243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -1271,8 +1258,8 @@
         <f aca="false">IF(C26+D26 &lt;= 10,C26+D26,10)</f>
         <v>2</v>
       </c>
-      <c r="F26" s="0"/>
-      <c r="G26" s="5" t="n">
+      <c r="F26" s="5"/>
+      <c r="G26" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H26" s="2" t="n">
@@ -1284,7 +1271,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -1302,7 +1289,7 @@
       <c r="F27" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G27" s="5" t="n">
+      <c r="G27" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H27" s="2" t="n">
@@ -1314,7 +1301,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
         <v>58</v>
       </c>
@@ -1329,8 +1316,8 @@
         <f aca="false">IF(C28+D28 &lt;= 10,C28+D28,10)</f>
         <v>2</v>
       </c>
-      <c r="F28" s="0"/>
-      <c r="G28" s="5" t="n">
+      <c r="F28" s="5"/>
+      <c r="G28" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H28" s="2" t="n">
@@ -1342,7 +1329,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
         <v>60</v>
       </c>
@@ -1362,7 +1349,7 @@
       <c r="F29" s="2" t="n">
         <v>8.25</v>
       </c>
-      <c r="G29" s="5" t="n">
+      <c r="G29" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H29" s="2" t="n">
@@ -1374,7 +1361,7 @@
         <v>8.1</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
         <v>62</v>
       </c>
@@ -1391,8 +1378,8 @@
         <f aca="false">IF(C30+D30 &lt;= 10,C30+D30,10)</f>
         <v>3.2</v>
       </c>
-      <c r="F30" s="0"/>
-      <c r="G30" s="5" t="n">
+      <c r="F30" s="5"/>
+      <c r="G30" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H30" s="2" t="n">
@@ -1404,7 +1391,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
         <v>64</v>
       </c>
@@ -1424,7 +1411,7 @@
       <c r="F31" s="2" t="n">
         <v>6.75</v>
       </c>
-      <c r="G31" s="5" t="n">
+      <c r="G31" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H31" s="2" t="n">
@@ -1436,7 +1423,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
         <v>66</v>
       </c>
@@ -1453,8 +1440,8 @@
         <f aca="false">IF(C32+D32 &lt;= 10,C32+D32,10)</f>
         <v>2</v>
       </c>
-      <c r="F32" s="0"/>
-      <c r="G32" s="5" t="n">
+      <c r="F32" s="5"/>
+      <c r="G32" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H32" s="2" t="n">
@@ -1466,7 +1453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
         <v>68</v>
       </c>
@@ -1481,8 +1468,8 @@
         <f aca="false">IF(C33+D33 &lt;= 10,C33+D33,10)</f>
         <v>2</v>
       </c>
-      <c r="F33" s="0"/>
-      <c r="G33" s="5" t="n">
+      <c r="F33" s="5"/>
+      <c r="G33" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H33" s="2" t="n">
@@ -1494,7 +1481,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
         <v>70</v>
       </c>
@@ -1514,7 +1501,7 @@
       <c r="F34" s="2" t="n">
         <v>5.6</v>
       </c>
-      <c r="G34" s="5" t="n">
+      <c r="G34" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H34" s="2" t="n">
@@ -1526,7 +1513,7 @@
         <v>6.65</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
         <v>72</v>
       </c>
@@ -1546,7 +1533,7 @@
       <c r="F35" s="2" t="n">
         <v>5.25</v>
       </c>
-      <c r="G35" s="5" t="n">
+      <c r="G35" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H35" s="2" t="n">
@@ -1558,7 +1545,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
@@ -1573,8 +1560,8 @@
         <f aca="false">IF(C36+D36 &lt;= 10,C36+D36,10)</f>
         <v>2</v>
       </c>
-      <c r="F36" s="0"/>
-      <c r="G36" s="5" t="n">
+      <c r="F36" s="5"/>
+      <c r="G36" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H36" s="2" t="n">
@@ -1586,7 +1573,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
         <v>76</v>
       </c>
@@ -1606,7 +1593,7 @@
       <c r="F37" s="2" t="n">
         <v>7.5</v>
       </c>
-      <c r="G37" s="5" t="n">
+      <c r="G37" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H37" s="2" t="n">
@@ -1618,7 +1605,7 @@
         <v>8.24</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
         <v>78</v>
       </c>
@@ -1638,7 +1625,7 @@
       <c r="F38" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="G38" s="5" t="n">
+      <c r="G38" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H38" s="2" t="n">
@@ -1650,7 +1637,7 @@
         <v>7.85</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
         <v>80</v>
       </c>
@@ -1670,7 +1657,7 @@
       <c r="F39" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="G39" s="5" t="n">
+      <c r="G39" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H39" s="2" t="n">
@@ -1682,7 +1669,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
         <v>82</v>
       </c>
@@ -1702,7 +1689,7 @@
       <c r="F40" s="2" t="n">
         <v>8.25</v>
       </c>
-      <c r="G40" s="5" t="n">
+      <c r="G40" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H40" s="2" t="n">
@@ -1714,7 +1701,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
         <v>84</v>
       </c>
@@ -1731,7 +1718,7 @@
         <f aca="false">IF(C41+D41 &lt;= 10,C41+D41,10)</f>
         <v>2</v>
       </c>
-      <c r="G41" s="5" t="n">
+      <c r="G41" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H41" s="2" t="n">
@@ -1743,7 +1730,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
         <v>86</v>
       </c>
@@ -1760,7 +1747,7 @@
         <f aca="false">IF(C42+D42 &lt;= 10,C42+D42,10)</f>
         <v>2.8</v>
       </c>
-      <c r="G42" s="5" t="n">
+      <c r="G42" s="6" t="n">
         <v>2</v>
       </c>
       <c r="H42" s="2" t="n">
@@ -1780,7 +1767,7 @@
     <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>6</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="3" operator="greaterThanOrEqual" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>6</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>